<commit_message>
remove db.py, add award field to person,work entities, cleanup
</commit_message>
<xml_diff>
--- a/app/db/faculty-Cornell-CS.xlsx
+++ b/app/db/faculty-Cornell-CS.xlsx
@@ -2275,12 +2275,18 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor rgb="FFFFFF00"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -2327,7 +2333,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="7">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -2341,6 +2347,18 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2364,8 +2382,12 @@
   </sheetPr>
   <dimension ref="A1:O123"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="J1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="O1" activeCellId="0" sqref="O1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="2" ySplit="1" topLeftCell="C92" activePane="bottomRight" state="frozen"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topRight" activeCell="C1" activeCellId="0" sqref="C1"/>
+      <selection pane="bottomLeft" activeCell="A92" activeCellId="0" sqref="A92"/>
+      <selection pane="bottomRight" activeCell="K99" activeCellId="0" sqref="K99"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -5480,35 +5502,35 @@
         <v>42</v>
       </c>
     </row>
-    <row r="99" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A99" s="1" t="s">
+    <row r="99" s="6" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A99" s="4" t="s">
         <v>599</v>
       </c>
-      <c r="B99" s="1" t="s">
+      <c r="B99" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="C99" s="1" t="s">
+      <c r="C99" s="4" t="s">
         <v>600</v>
       </c>
-      <c r="D99" s="1" t="s">
+      <c r="D99" s="4" t="s">
         <v>108</v>
       </c>
-      <c r="E99" s="1" t="s">
+      <c r="E99" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="F99" s="1" t="s">
+      <c r="F99" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="G99" s="1" t="s">
+      <c r="G99" s="4" t="s">
         <v>601</v>
       </c>
-      <c r="H99" s="3" t="s">
+      <c r="H99" s="5" t="s">
         <v>602</v>
       </c>
-      <c r="I99" s="3" t="s">
+      <c r="I99" s="5" t="s">
         <v>603</v>
       </c>
-      <c r="N99" s="1" t="s">
+      <c r="N99" s="4" t="s">
         <v>32</v>
       </c>
     </row>

</xml_diff>